<commit_message>
updated event checklist with more items
</commit_message>
<xml_diff>
--- a/assets/EventChecklist.xlsx
+++ b/assets/EventChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sql-saturday-website\docs\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F15BB24-8BF5-4EF9-9725-13D9053D481E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE2B7CA-5B7E-45B6-9469-1DAD86B49BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6FE3E817-6BA9-4291-A0BA-63087DBF9607}"/>
+    <workbookView xWindow="7050" yWindow="360" windowWidth="20760" windowHeight="14250" xr2:uid="{6FE3E817-6BA9-4291-A0BA-63087DBF9607}"/>
   </bookViews>
   <sheets>
     <sheet name="New Event Checklist" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>New SQL Saturday Event</t>
   </si>
@@ -78,49 +78,126 @@
     <t>Event Description</t>
   </si>
   <si>
-    <t xml:space="preserve">
-This is the first annual Data Saturday organized by the Maltese community and focused on the Maltese Market needs.
+    <t>CFP URL</t>
+  </si>
+  <si>
+    <t>CFP End Date</t>
+  </si>
+  <si>
+    <t>April 1, 2021</t>
+  </si>
+  <si>
+    <t>Organizer Name</t>
+  </si>
+  <si>
+    <t>Andy Warren and Steve Jones</t>
+  </si>
+  <si>
+    <t>Contact Email</t>
+  </si>
+  <si>
+    <t>support@sqlsaturday.com</t>
+  </si>
+  <si>
+    <t>Sponsor Plan URL</t>
+  </si>
+  <si>
+    <t>Logo URL (&lt;200x100)</t>
+  </si>
+  <si>
+    <t>Logo URL (full size for event page)</t>
+  </si>
+  <si>
+    <t>For new events, fill in values in the "C" column and then submit this to the SQL Saturday site.</t>
+  </si>
+  <si>
+    <t>Event Time</t>
+  </si>
+  <si>
+    <t>0900 MST - 0500 MST</t>
+  </si>
+  <si>
+    <t>Using Rooms for Virtual?</t>
+  </si>
+  <si>
+    <t>Precons?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>This will enable a menu item and section for precons</t>
+  </si>
+  <si>
+    <t>This enables the Rooms section</t>
+  </si>
+  <si>
+    <t>Twitter account for organizer/group</t>
+  </si>
+  <si>
+    <t>denversql</t>
+  </si>
+  <si>
+    <t>@denversql</t>
+  </si>
+  <si>
+    <t>https://2022datasqlsatla.eventbrite.com/</t>
+  </si>
+  <si>
+    <t>This is the first annual Data Saturday organized by the Maltese community and focused on the Maltese Market needs.
 This is a free training day full of information about Microsoft Data Platform brought to us by the best international speakers available
 Due to the COVID pandemic, this event will be held online.</t>
   </si>
   <si>
-    <t>CFP URL</t>
-  </si>
-  <si>
-    <t>CFP End Date</t>
-  </si>
-  <si>
-    <t>April 1, 2021</t>
-  </si>
-  <si>
-    <t>Organizer Name</t>
-  </si>
-  <si>
-    <t>Andy Warren and Steve Jones</t>
-  </si>
-  <si>
-    <t>Contact Email</t>
-  </si>
-  <si>
-    <t>support@sqlsaturday.com</t>
-  </si>
-  <si>
-    <t>Sponsor Plan URL</t>
-  </si>
-  <si>
-    <t>Logo URL (&lt;200x100)</t>
-  </si>
-  <si>
-    <t>Logo URL (full size for event page)</t>
-  </si>
-  <si>
-    <t>For new events, fill in values in the "C" column and then submit this to the SQL Saturday site.</t>
-  </si>
-  <si>
-    <t>Event Time</t>
-  </si>
-  <si>
-    <t>0900 MST - 0500 MST</t>
+    <t>Event Capacity</t>
+  </si>
+  <si>
+    <t>numerical display</t>
+  </si>
+  <si>
+    <t>If you have a limit, enter 120-130% of the limit</t>
+  </si>
+  <si>
+    <t>Contact URL</t>
+  </si>
+  <si>
+    <t>http://www.denversql.org</t>
+  </si>
+  <si>
+    <t>URL shown</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Everything after youtube domain, like: channel/UCj37MpcNm-2uVOetqiij9PQ/videos</t>
+  </si>
+  <si>
+    <t>Linkedin URL</t>
+  </si>
+  <si>
+    <t>link to youtube channel</t>
+  </si>
+  <si>
+    <t>link to linkedin group</t>
+  </si>
+  <si>
+    <t>Sponsorship plan</t>
+  </si>
+  <si>
+    <t>HTML for sponsorship plans. Steal from another event</t>
+  </si>
+  <si>
+    <t>Precon details</t>
+  </si>
+  <si>
+    <t>HTML of precon details</t>
   </si>
 </sst>
 </file>
@@ -192,7 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -213,6 +290,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,19 +637,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3206B0-269B-4FCF-90F0-0C82AEB6F3F4}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="51.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -582,7 +662,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -643,7 +723,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="3"/>
@@ -652,41 +732,39 @@
         <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="str">
-        <f t="shared" ref="A9:A19" si="0">IF(ISTEXT(C9), "X", " ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="10">
-        <f t="shared" ref="E9:E19" si="1">+C9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A10:A23" si="0">IF(ISTEXT(C10), "X", " ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="5"/>
       <c r="E10" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>17</v>
+        <f t="shared" ref="E10:E22" si="1">+C10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -695,14 +773,17 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
@@ -710,49 +791,49 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12" s="7"/>
       <c r="E12" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="7"/>
       <c r="E13" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C14" s="7"/>
       <c r="E14" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>19</v>
+      <c r="F14" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -761,15 +842,15 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="7"/>
       <c r="E15" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>21</v>
+      <c r="F15" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -778,50 +859,51 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="7"/>
       <c r="E16" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="E17" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="7"/>
+      <c r="E17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="E18" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="7"/>
+      <c r="E18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="E19" s="10">
         <f t="shared" si="1"/>
@@ -831,33 +913,124 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
       <c r="C20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="7"/>
+      <c r="E21" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
       <c r="C22" s="7"/>
+      <c r="E22" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
       <c r="C23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
       <c r="C24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
       <c r="C25" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
       <c r="C26" s="7"/>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
       <c r="C27" s="7"/>
+      <c r="E27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6">
@@ -876,7 +1049,7 @@
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A18">
+  <conditionalFormatting sqref="A10:A22">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
@@ -884,7 +1057,7 @@
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
+  <conditionalFormatting sqref="A8:A9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>""""""</formula>
     </cfRule>
@@ -893,9 +1066,12 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F15" r:id="rId1" xr:uid="{A1038F06-E7F0-41F5-8670-A25ADE817599}"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{0CFE5740-6F17-49A3-AEC5-2C22109342A9}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{A1038F06-E7F0-41F5-8670-A25ADE817599}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{9FC7318D-C12A-45EE-8971-EC5FB42066FF}"/>
+    <hyperlink ref="F17" r:id="rId4" xr:uid="{AD7C9498-3A83-4EE5-9539-6DC8C44FB8AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>